<commit_message>
I want to break free
</commit_message>
<xml_diff>
--- a/LR3/table_1_92.xlsx
+++ b/LR3/table_1_92.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79196\Desktop\ИТ\LR3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030D57E0-7EBE-4F9A-B882-FA6F6FAF1599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816608DF-16D2-4499-BE4B-F4BD73BAF66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{5E67452D-B42B-4A17-B44C-645558D96547}"/>
   </bookViews>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -587,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D94C37-CB8B-4599-B4B1-AB35136A6C63}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -656,8 +659,8 @@
         <v>1</v>
       </c>
       <c r="C3" s="3">
-        <f>A1</f>
-        <v>92</v>
+        <f>70</f>
+        <v>70</v>
       </c>
       <c r="D3" s="3">
         <f>$A$1*1.1</f>
@@ -665,7 +668,7 @@
       </c>
       <c r="E3" s="3">
         <f>C3*D3</f>
-        <v>9310.4</v>
+        <v>7084</v>
       </c>
       <c r="F3" s="4">
         <v>44813</v>
@@ -686,7 +689,7 @@
       </c>
       <c r="K3" s="3">
         <f>E3+J3</f>
-        <v>9310.4</v>
+        <v>7084</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -699,7 +702,7 @@
       </c>
       <c r="C4" s="3">
         <f>C3-0.5</f>
-        <v>91.5</v>
+        <v>69.5</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ref="D4:D34" si="0">$A$1*1.1</f>
@@ -707,7 +710,7 @@
       </c>
       <c r="E4" s="3">
         <f t="shared" ref="E4:E38" si="1">C4*D4</f>
-        <v>9259.8000000000011</v>
+        <v>7033.4000000000005</v>
       </c>
       <c r="F4" s="4">
         <f>F3</f>
@@ -730,7 +733,7 @@
       </c>
       <c r="K4" s="3">
         <f t="shared" ref="K4:K38" si="4">E4+J4</f>
-        <v>9259.8000000000011</v>
+        <v>7033.4000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -743,7 +746,7 @@
       </c>
       <c r="C5" s="3">
         <f t="shared" ref="C5:C38" si="6">C4-0.5</f>
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
@@ -751,7 +754,7 @@
       </c>
       <c r="E5" s="3">
         <f t="shared" si="1"/>
-        <v>9209.2000000000007</v>
+        <v>6982.8</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" ref="F5:F38" si="7">F4</f>
@@ -774,7 +777,7 @@
       </c>
       <c r="K5" s="3">
         <f t="shared" si="4"/>
-        <v>9209.2000000000007</v>
+        <v>6982.8</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -787,7 +790,7 @@
       </c>
       <c r="C6" s="3">
         <f t="shared" si="6"/>
-        <v>90.5</v>
+        <v>68.5</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
@@ -795,7 +798,7 @@
       </c>
       <c r="E6" s="3">
         <f t="shared" si="1"/>
-        <v>9158.6</v>
+        <v>6932.2</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="7"/>
@@ -818,7 +821,7 @@
       </c>
       <c r="K6" s="3">
         <f t="shared" si="4"/>
-        <v>9158.6</v>
+        <v>6932.2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -831,7 +834,7 @@
       </c>
       <c r="C7" s="3">
         <f t="shared" si="6"/>
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
@@ -839,7 +842,7 @@
       </c>
       <c r="E7" s="3">
         <f t="shared" si="1"/>
-        <v>9108</v>
+        <v>6881.6</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="7"/>
@@ -862,7 +865,7 @@
       </c>
       <c r="K7" s="3">
         <f t="shared" si="4"/>
-        <v>9108</v>
+        <v>6881.6</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -875,7 +878,7 @@
       </c>
       <c r="C8" s="3">
         <f t="shared" si="6"/>
-        <v>89.5</v>
+        <v>67.5</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
@@ -883,7 +886,7 @@
       </c>
       <c r="E8" s="3">
         <f t="shared" si="1"/>
-        <v>9057.4</v>
+        <v>6831</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="7"/>
@@ -906,7 +909,7 @@
       </c>
       <c r="K8" s="3">
         <f t="shared" si="4"/>
-        <v>9057.4</v>
+        <v>6831</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -919,7 +922,7 @@
       </c>
       <c r="C9" s="3">
         <f t="shared" si="6"/>
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
@@ -927,7 +930,7 @@
       </c>
       <c r="E9" s="3">
         <f t="shared" si="1"/>
-        <v>9006.8000000000011</v>
+        <v>6780.4000000000005</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="7"/>
@@ -950,7 +953,7 @@
       </c>
       <c r="K9" s="3">
         <f t="shared" si="4"/>
-        <v>9006.8000000000011</v>
+        <v>6780.4000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -963,7 +966,7 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" si="6"/>
-        <v>88.5</v>
+        <v>66.5</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
@@ -971,7 +974,7 @@
       </c>
       <c r="E10" s="3">
         <f t="shared" si="1"/>
-        <v>8956.2000000000007</v>
+        <v>6729.8</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="7"/>
@@ -994,7 +997,7 @@
       </c>
       <c r="K10" s="3">
         <f t="shared" si="4"/>
-        <v>8956.2000000000007</v>
+        <v>6729.8</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1007,7 +1010,7 @@
       </c>
       <c r="C11" s="3">
         <f t="shared" si="6"/>
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
@@ -1015,7 +1018,7 @@
       </c>
       <c r="E11" s="3">
         <f t="shared" si="1"/>
-        <v>8905.6</v>
+        <v>6679.2</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="7"/>
@@ -1038,7 +1041,7 @@
       </c>
       <c r="K11" s="3">
         <f t="shared" si="4"/>
-        <v>8905.6</v>
+        <v>6679.2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1051,7 +1054,7 @@
       </c>
       <c r="C12" s="3">
         <f t="shared" si="6"/>
-        <v>87.5</v>
+        <v>65.5</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
@@ -1059,7 +1062,7 @@
       </c>
       <c r="E12" s="3">
         <f t="shared" si="1"/>
-        <v>8855</v>
+        <v>6628.6</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="7"/>
@@ -1082,7 +1085,7 @@
       </c>
       <c r="K12" s="3">
         <f t="shared" si="4"/>
-        <v>8865</v>
+        <v>6638.6</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1095,7 +1098,7 @@
       </c>
       <c r="C13" s="3">
         <f t="shared" si="6"/>
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" si="0"/>
@@ -1103,7 +1106,7 @@
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>8804.4</v>
+        <v>6578</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="7"/>
@@ -1126,7 +1129,7 @@
       </c>
       <c r="K13" s="3">
         <f t="shared" si="4"/>
-        <v>8824.4</v>
+        <v>6598</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1139,7 +1142,7 @@
       </c>
       <c r="C14" s="3">
         <f t="shared" si="6"/>
-        <v>86.5</v>
+        <v>64.5</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" si="0"/>
@@ -1147,7 +1150,7 @@
       </c>
       <c r="E14" s="3">
         <f t="shared" si="1"/>
-        <v>8753.8000000000011</v>
+        <v>6527.4000000000005</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" si="7"/>
@@ -1170,7 +1173,7 @@
       </c>
       <c r="K14" s="3">
         <f t="shared" si="4"/>
-        <v>8783.8000000000011</v>
+        <v>6557.4000000000005</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1183,7 +1186,7 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" si="6"/>
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" si="0"/>
@@ -1191,7 +1194,7 @@
       </c>
       <c r="E15" s="3">
         <f t="shared" si="1"/>
-        <v>8703.2000000000007</v>
+        <v>6476.8</v>
       </c>
       <c r="F15" s="4">
         <f t="shared" si="7"/>
@@ -1214,7 +1217,7 @@
       </c>
       <c r="K15" s="3">
         <f t="shared" si="4"/>
-        <v>8743.2000000000007</v>
+        <v>6516.8</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1227,7 +1230,7 @@
       </c>
       <c r="C16" s="3">
         <f t="shared" si="6"/>
-        <v>85.5</v>
+        <v>63.5</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" si="0"/>
@@ -1235,7 +1238,7 @@
       </c>
       <c r="E16" s="3">
         <f t="shared" si="1"/>
-        <v>8652.6</v>
+        <v>6426.2</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="7"/>
@@ -1258,7 +1261,7 @@
       </c>
       <c r="K16" s="3">
         <f t="shared" si="4"/>
-        <v>8702.6</v>
+        <v>6476.2</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -1271,7 +1274,7 @@
       </c>
       <c r="C17" s="3">
         <f t="shared" si="6"/>
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="0"/>
@@ -1279,7 +1282,7 @@
       </c>
       <c r="E17" s="3">
         <f t="shared" si="1"/>
-        <v>8602</v>
+        <v>6375.6</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="7"/>
@@ -1302,7 +1305,7 @@
       </c>
       <c r="K17" s="3">
         <f t="shared" si="4"/>
-        <v>8662</v>
+        <v>6435.6</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -1315,7 +1318,7 @@
       </c>
       <c r="C18" s="3">
         <f t="shared" si="6"/>
-        <v>84.5</v>
+        <v>62.5</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" si="0"/>
@@ -1323,7 +1326,7 @@
       </c>
       <c r="E18" s="3">
         <f t="shared" si="1"/>
-        <v>8551.4</v>
+        <v>6325</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="7"/>
@@ -1346,7 +1349,7 @@
       </c>
       <c r="K18" s="3">
         <f t="shared" si="4"/>
-        <v>8621.4</v>
+        <v>6395</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -1359,7 +1362,7 @@
       </c>
       <c r="C19" s="3">
         <f t="shared" si="6"/>
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" si="0"/>
@@ -1367,7 +1370,7 @@
       </c>
       <c r="E19" s="3">
         <f t="shared" si="1"/>
-        <v>8500.8000000000011</v>
+        <v>6274.4000000000005</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" si="7"/>
@@ -1390,7 +1393,7 @@
       </c>
       <c r="K19" s="3">
         <f t="shared" si="4"/>
-        <v>8580.8000000000011</v>
+        <v>6354.4000000000005</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1403,7 +1406,7 @@
       </c>
       <c r="C20" s="3">
         <f t="shared" si="6"/>
-        <v>83.5</v>
+        <v>61.5</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" si="0"/>
@@ -1411,7 +1414,7 @@
       </c>
       <c r="E20" s="3">
         <f t="shared" si="1"/>
-        <v>8450.2000000000007</v>
+        <v>6223.8</v>
       </c>
       <c r="F20" s="4">
         <f t="shared" si="7"/>
@@ -1434,7 +1437,7 @@
       </c>
       <c r="K20" s="3">
         <f t="shared" si="4"/>
-        <v>8540.2000000000007</v>
+        <v>6313.8</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1447,7 +1450,7 @@
       </c>
       <c r="C21" s="3">
         <f t="shared" si="6"/>
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="0"/>
@@ -1455,7 +1458,7 @@
       </c>
       <c r="E21" s="3">
         <f t="shared" si="1"/>
-        <v>8399.6</v>
+        <v>6173.2</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" si="7"/>
@@ -1478,7 +1481,7 @@
       </c>
       <c r="K21" s="3">
         <f t="shared" si="4"/>
-        <v>8499.6</v>
+        <v>6273.2</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -1491,7 +1494,7 @@
       </c>
       <c r="C22" s="3">
         <f t="shared" si="6"/>
-        <v>82.5</v>
+        <v>60.5</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" si="0"/>
@@ -1499,7 +1502,7 @@
       </c>
       <c r="E22" s="3">
         <f t="shared" si="1"/>
-        <v>8349</v>
+        <v>6122.6</v>
       </c>
       <c r="F22" s="4">
         <f t="shared" si="7"/>
@@ -1522,7 +1525,7 @@
       </c>
       <c r="K22" s="3">
         <f t="shared" si="4"/>
-        <v>8459</v>
+        <v>6232.6</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -1535,7 +1538,7 @@
       </c>
       <c r="C23" s="3">
         <f t="shared" si="6"/>
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" si="0"/>
@@ -1543,7 +1546,7 @@
       </c>
       <c r="E23" s="3">
         <f t="shared" si="1"/>
-        <v>8298.4</v>
+        <v>6072</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" si="7"/>
@@ -1566,7 +1569,7 @@
       </c>
       <c r="K23" s="3">
         <f t="shared" si="4"/>
-        <v>8418.4</v>
+        <v>6192</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -1579,7 +1582,7 @@
       </c>
       <c r="C24" s="3">
         <f t="shared" si="6"/>
-        <v>81.5</v>
+        <v>59.5</v>
       </c>
       <c r="D24" s="3">
         <f t="shared" si="0"/>
@@ -1587,7 +1590,7 @@
       </c>
       <c r="E24" s="3">
         <f t="shared" si="1"/>
-        <v>8247.8000000000011</v>
+        <v>6021.4000000000005</v>
       </c>
       <c r="F24" s="4">
         <f t="shared" si="7"/>
@@ -1610,7 +1613,7 @@
       </c>
       <c r="K24" s="3">
         <f t="shared" si="4"/>
-        <v>8377.8000000000011</v>
+        <v>6151.4000000000005</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -1623,7 +1626,7 @@
       </c>
       <c r="C25" s="3">
         <f t="shared" si="6"/>
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" si="0"/>
@@ -1631,7 +1634,7 @@
       </c>
       <c r="E25" s="3">
         <f t="shared" si="1"/>
-        <v>8197.2000000000007</v>
+        <v>5970.8</v>
       </c>
       <c r="F25" s="4">
         <f t="shared" si="7"/>
@@ -1654,7 +1657,7 @@
       </c>
       <c r="K25" s="3">
         <f t="shared" si="4"/>
-        <v>8337.2000000000007</v>
+        <v>6110.8</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -1667,7 +1670,7 @@
       </c>
       <c r="C26" s="3">
         <f t="shared" si="6"/>
-        <v>80.5</v>
+        <v>58.5</v>
       </c>
       <c r="D26" s="3">
         <f t="shared" si="0"/>
@@ -1675,7 +1678,7 @@
       </c>
       <c r="E26" s="3">
         <f t="shared" si="1"/>
-        <v>8146.6</v>
+        <v>5920.2</v>
       </c>
       <c r="F26" s="4">
         <f t="shared" si="7"/>
@@ -1698,7 +1701,7 @@
       </c>
       <c r="K26" s="3">
         <f t="shared" si="4"/>
-        <v>8296.6</v>
+        <v>6070.2</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1711,7 +1714,7 @@
       </c>
       <c r="C27" s="3">
         <f t="shared" si="6"/>
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="D27" s="3">
         <f t="shared" si="0"/>
@@ -1719,7 +1722,7 @@
       </c>
       <c r="E27" s="3">
         <f t="shared" si="1"/>
-        <v>8096</v>
+        <v>5869.6</v>
       </c>
       <c r="F27" s="4">
         <f t="shared" si="7"/>
@@ -1742,7 +1745,7 @@
       </c>
       <c r="K27" s="3">
         <f t="shared" si="4"/>
-        <v>8256</v>
+        <v>6029.6</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1755,7 +1758,7 @@
       </c>
       <c r="C28" s="3">
         <f t="shared" si="6"/>
-        <v>79.5</v>
+        <v>57.5</v>
       </c>
       <c r="D28" s="3">
         <f t="shared" si="0"/>
@@ -1763,7 +1766,7 @@
       </c>
       <c r="E28" s="3">
         <f t="shared" si="1"/>
-        <v>8045.4000000000005</v>
+        <v>5819</v>
       </c>
       <c r="F28" s="4">
         <f t="shared" si="7"/>
@@ -1786,7 +1789,7 @@
       </c>
       <c r="K28" s="3">
         <f t="shared" si="4"/>
-        <v>8215.4000000000015</v>
+        <v>5989</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -1799,7 +1802,7 @@
       </c>
       <c r="C29" s="3">
         <f t="shared" si="6"/>
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" si="0"/>
@@ -1807,7 +1810,7 @@
       </c>
       <c r="E29" s="3">
         <f t="shared" si="1"/>
-        <v>7994.8</v>
+        <v>5768.4000000000005</v>
       </c>
       <c r="F29" s="4">
         <f t="shared" si="7"/>
@@ -1830,7 +1833,7 @@
       </c>
       <c r="K29" s="3">
         <f t="shared" si="4"/>
-        <v>8174.8</v>
+        <v>5948.4000000000005</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -1843,7 +1846,7 @@
       </c>
       <c r="C30" s="3">
         <f t="shared" si="6"/>
-        <v>78.5</v>
+        <v>56.5</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" si="0"/>
@@ -1851,7 +1854,7 @@
       </c>
       <c r="E30" s="3">
         <f t="shared" si="1"/>
-        <v>7944.2</v>
+        <v>5717.8</v>
       </c>
       <c r="F30" s="4">
         <f t="shared" si="7"/>
@@ -1874,7 +1877,7 @@
       </c>
       <c r="K30" s="3">
         <f t="shared" si="4"/>
-        <v>8134.2</v>
+        <v>5907.8</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -1887,7 +1890,7 @@
       </c>
       <c r="C31" s="3">
         <f t="shared" si="6"/>
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="D31" s="3">
         <f t="shared" si="0"/>
@@ -1895,7 +1898,7 @@
       </c>
       <c r="E31" s="3">
         <f t="shared" si="1"/>
-        <v>7893.6</v>
+        <v>5667.2</v>
       </c>
       <c r="F31" s="4">
         <f t="shared" si="7"/>
@@ -1918,7 +1921,7 @@
       </c>
       <c r="K31" s="3">
         <f t="shared" si="4"/>
-        <v>8093.6</v>
+        <v>5867.2</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -1931,7 +1934,7 @@
       </c>
       <c r="C32" s="3">
         <f t="shared" si="6"/>
-        <v>77.5</v>
+        <v>55.5</v>
       </c>
       <c r="D32" s="3">
         <f t="shared" si="0"/>
@@ -1939,7 +1942,7 @@
       </c>
       <c r="E32" s="3">
         <f t="shared" si="1"/>
-        <v>7843</v>
+        <v>5616.6</v>
       </c>
       <c r="F32" s="4">
         <f t="shared" si="7"/>
@@ -1962,7 +1965,7 @@
       </c>
       <c r="K32" s="3">
         <f t="shared" si="4"/>
-        <v>8053</v>
+        <v>5826.6</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -1975,7 +1978,7 @@
       </c>
       <c r="C33" s="3">
         <f t="shared" si="6"/>
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="D33" s="3">
         <f t="shared" si="0"/>
@@ -1983,7 +1986,7 @@
       </c>
       <c r="E33" s="3">
         <f t="shared" si="1"/>
-        <v>7792.4000000000005</v>
+        <v>5566</v>
       </c>
       <c r="F33" s="4">
         <f t="shared" si="7"/>
@@ -2006,7 +2009,7 @@
       </c>
       <c r="K33" s="3">
         <f t="shared" si="4"/>
-        <v>8012.4000000000005</v>
+        <v>5786</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -2019,7 +2022,7 @@
       </c>
       <c r="C34" s="3">
         <f t="shared" si="6"/>
-        <v>76.5</v>
+        <v>54.5</v>
       </c>
       <c r="D34" s="3">
         <f t="shared" si="0"/>
@@ -2027,7 +2030,7 @@
       </c>
       <c r="E34" s="3">
         <f t="shared" si="1"/>
-        <v>7741.8</v>
+        <v>5515.4000000000005</v>
       </c>
       <c r="F34" s="4">
         <f t="shared" si="7"/>
@@ -2050,7 +2053,7 @@
       </c>
       <c r="K34" s="3">
         <f t="shared" si="4"/>
-        <v>7971.8</v>
+        <v>5745.4000000000005</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -2063,7 +2066,7 @@
       </c>
       <c r="C35" s="3">
         <f t="shared" si="6"/>
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D35" s="3">
         <f>$A$1*1.1/2</f>
@@ -2071,7 +2074,7 @@
       </c>
       <c r="E35" s="3">
         <f t="shared" si="1"/>
-        <v>3845.6</v>
+        <v>2732.4</v>
       </c>
       <c r="F35" s="4">
         <f t="shared" si="7"/>
@@ -2094,7 +2097,7 @@
       </c>
       <c r="K35" s="3">
         <f t="shared" si="4"/>
-        <v>4085.6</v>
+        <v>2972.4</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -2107,7 +2110,7 @@
       </c>
       <c r="C36" s="3">
         <f t="shared" si="6"/>
-        <v>75.5</v>
+        <v>53.5</v>
       </c>
       <c r="D36" s="3">
         <f t="shared" ref="D36:D38" si="9">$A$1*1.1/2</f>
@@ -2115,7 +2118,7 @@
       </c>
       <c r="E36" s="3">
         <f t="shared" si="1"/>
-        <v>3820.3</v>
+        <v>2707.1</v>
       </c>
       <c r="F36" s="4">
         <f t="shared" si="7"/>
@@ -2138,7 +2141,7 @@
       </c>
       <c r="K36" s="3">
         <f t="shared" si="4"/>
-        <v>4070.3</v>
+        <v>2957.1</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -2151,7 +2154,7 @@
       </c>
       <c r="C37" s="3">
         <f t="shared" si="6"/>
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="D37" s="3">
         <f t="shared" si="9"/>
@@ -2159,7 +2162,7 @@
       </c>
       <c r="E37" s="3">
         <f t="shared" si="1"/>
-        <v>3795</v>
+        <v>2681.8</v>
       </c>
       <c r="F37" s="4">
         <f t="shared" si="7"/>
@@ -2182,7 +2185,7 @@
       </c>
       <c r="K37" s="3">
         <f t="shared" si="4"/>
-        <v>4055</v>
+        <v>2941.8</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -2195,7 +2198,7 @@
       </c>
       <c r="C38" s="3">
         <f t="shared" si="6"/>
-        <v>74.5</v>
+        <v>52.5</v>
       </c>
       <c r="D38" s="3">
         <f t="shared" si="9"/>
@@ -2203,7 +2206,7 @@
       </c>
       <c r="E38" s="3">
         <f t="shared" si="1"/>
-        <v>3769.7000000000003</v>
+        <v>2656.5</v>
       </c>
       <c r="F38" s="4">
         <f t="shared" si="7"/>
@@ -2226,7 +2229,7 @@
       </c>
       <c r="K38" s="3">
         <f t="shared" si="4"/>
-        <v>4039.7000000000003</v>
+        <v>2926.5</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2235,7 +2238,7 @@
       </c>
       <c r="C40" s="5">
         <f>ROUNDDOWN(SUM(K3:K38),0)</f>
-        <v>291845</v>
+        <v>216148</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -2244,7 +2247,7 @@
       </c>
       <c r="C41" s="3">
         <f>AVERAGE(C3:C38)</f>
-        <v>83.25</v>
+        <v>61.25</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -2262,7 +2265,7 @@
       </c>
       <c r="C43" s="3">
         <f>MAX(K3:K38)</f>
-        <v>9310.4</v>
+        <v>7084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>